<commit_message>
files for app with corrections
</commit_message>
<xml_diff>
--- a/sub_pro_1_hass_land_price_app/processed_tables/hass_satellite_combined_2015_to_20XX.xlsx
+++ b/sub_pro_1_hass_land_price_app/processed_tables/hass_satellite_combined_2015_to_20XX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\shiny_app_dev\sub_pro_1_hass_land_price_app\processed_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA8B336-4DB1-4861-9730-BEF547438705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB888E99-3254-43B0-B2E3-EC9232423EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="329" xr2:uid="{F6B0FCA6-F3F3-43C0-91BB-C36AABF9161E}"/>
+    <workbookView xWindow="6560" yWindow="130" windowWidth="9050" windowHeight="10070" tabRatio="329" xr2:uid="{F6B0FCA6-F3F3-43C0-91BB-C36AABF9161E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="21">
   <si>
     <t>Athi River</t>
   </si>
@@ -88,75 +88,6 @@
   </si>
   <si>
     <t>75th Percentile</t>
-  </si>
-  <si>
-    <t>21,100,000 8,000,000 30,000,000</t>
-  </si>
-  <si>
-    <t>25,100,000 14,800,000 28,800,000</t>
-  </si>
-  <si>
-    <t>49,700,000 30,000,000 64,000,000</t>
-  </si>
-  <si>
-    <t>18,200,000 10,200,000 20,000,000</t>
-  </si>
-  <si>
-    <t>26,100,000 16,000,000 32,100,000</t>
-  </si>
-  <si>
-    <t>45,400,000 25,000,000 60,000,000</t>
-  </si>
-  <si>
-    <t>36,900,000 22,400,000 48,000,000</t>
-  </si>
-  <si>
-    <t>37,200,000 22,000,000 45,400,000</t>
-  </si>
-  <si>
-    <t>30,000,000 42,000,000</t>
-  </si>
-  <si>
-    <t>19,800,000 34,000,000</t>
-  </si>
-  <si>
-    <t>25,000,000 37,900,000</t>
-  </si>
-  <si>
-    <t>21,400,000 10,000,000 30,000,000</t>
-  </si>
-  <si>
-    <t>25,500,000 17,600,000 30,000,000</t>
-  </si>
-  <si>
-    <t>48,700,000 28,800,000 60,000,000</t>
-  </si>
-  <si>
-    <t>18,700,000 11,100,000 20,800,000</t>
-  </si>
-  <si>
-    <t>26,900,000 18,400,000 32,000,000</t>
-  </si>
-  <si>
-    <t>46,900,000 30,000,000 60,000,000</t>
-  </si>
-  <si>
-    <t>36,200,000 23,000,000 48,000,000</t>
-  </si>
-  <si>
-    <t>28,500,000 15,000,000 35,000,000</t>
-  </si>
-  <si>
-    <t>38,100,000 22,600,000 45,000,000</t>
-  </si>
-  <si>
-    <t>32,000,000 42,000,000</t>
-  </si>
-  <si>
-    <t>19,800,000 33,000,000</t>
-  </si>
-  <si>
-    <t>27,000,000 40,000,000</t>
   </si>
 </sst>
 </file>
@@ -239,7 +170,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -269,7 +200,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -591,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC70402-8CDC-4196-A23D-FFEAA0C5A692}">
-  <dimension ref="A1:G607"/>
+  <dimension ref="A1:I607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A593" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G607" sqref="G607"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E161" sqref="E161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -604,6 +534,7 @@
     <col min="4" max="4" width="16.90625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.08984375" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1456,12 +1387,16 @@
       <c r="C43" s="1">
         <v>2</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="D43" s="9">
+        <v>21100000</v>
+      </c>
+      <c r="E43" s="9">
+        <v>8000000</v>
+      </c>
+      <c r="F43" s="9">
+        <v>30000000</v>
+      </c>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
@@ -1473,12 +1408,16 @@
       <c r="C44" s="1">
         <v>3</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" t="s">
-        <v>32</v>
-      </c>
+      <c r="D44" s="9">
+        <v>21400000</v>
+      </c>
+      <c r="E44" s="9">
+        <v>10000000</v>
+      </c>
+      <c r="F44" s="9">
+        <v>30000000</v>
+      </c>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
@@ -2310,12 +2249,16 @@
       <c r="C86" s="1">
         <v>2</v>
       </c>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="D86" s="9">
+        <v>25100000</v>
+      </c>
+      <c r="E86" s="9">
+        <v>14800000</v>
+      </c>
+      <c r="F86" s="9">
+        <v>28800000</v>
+      </c>
+      <c r="G86" s="15"/>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
@@ -2327,12 +2270,16 @@
       <c r="C87" s="1">
         <v>3</v>
       </c>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="D87" s="9">
+        <v>25500000</v>
+      </c>
+      <c r="E87" s="9">
+        <v>17600000</v>
+      </c>
+      <c r="F87" s="9">
+        <v>30000000</v>
+      </c>
+      <c r="G87" s="15"/>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
@@ -3164,12 +3111,16 @@
       <c r="C129" s="1">
         <v>2</v>
       </c>
-      <c r="D129" s="9"/>
-      <c r="E129" s="9"/>
-      <c r="F129" s="9"/>
-      <c r="G129" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="D129" s="9">
+        <v>49700000</v>
+      </c>
+      <c r="E129" s="9">
+        <v>30000000</v>
+      </c>
+      <c r="F129" s="9">
+        <v>64000000</v>
+      </c>
+      <c r="G129" s="15"/>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="1" t="s">
@@ -3181,12 +3132,16 @@
       <c r="C130" s="1">
         <v>3</v>
       </c>
-      <c r="D130" s="9"/>
-      <c r="E130" s="9"/>
-      <c r="F130" s="9"/>
-      <c r="G130" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="D130" s="9">
+        <v>48700000</v>
+      </c>
+      <c r="E130" s="9">
+        <v>28800000</v>
+      </c>
+      <c r="F130" s="9">
+        <v>60000000</v>
+      </c>
+      <c r="G130" s="15"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="1" t="s">
@@ -3788,7 +3743,7 @@
         <v>12800000</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:9">
       <c r="A161" s="1" t="s">
         <v>4</v>
       </c>
@@ -3808,7 +3763,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:9">
       <c r="A162" s="1" t="s">
         <v>4</v>
       </c>
@@ -3828,7 +3783,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:9">
       <c r="A163" s="1" t="s">
         <v>4</v>
       </c>
@@ -3848,7 +3803,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:9">
       <c r="A164" s="1" t="s">
         <v>4</v>
       </c>
@@ -3862,13 +3817,13 @@
         <v>9800000</v>
       </c>
       <c r="E164" s="9">
-        <v>9800000</v>
+        <v>4000000</v>
       </c>
       <c r="F164" s="9">
         <v>14400000</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:9">
       <c r="A165" s="1" t="s">
         <v>4</v>
       </c>
@@ -3888,7 +3843,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:9">
       <c r="A166" s="1" t="s">
         <v>4</v>
       </c>
@@ -3908,7 +3863,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:9">
       <c r="A167" s="1" t="s">
         <v>4</v>
       </c>
@@ -3928,7 +3883,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:9">
       <c r="A168" s="1" t="s">
         <v>4</v>
       </c>
@@ -3948,7 +3903,7 @@
         <v>14400000</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:9">
       <c r="A169" s="1" t="s">
         <v>4</v>
       </c>
@@ -3968,7 +3923,7 @@
         <v>16600000</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:9">
       <c r="A170" s="1" t="s">
         <v>4</v>
       </c>
@@ -3988,7 +3943,7 @@
         <v>16800000</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:9">
       <c r="A171" s="1" t="s">
         <v>4</v>
       </c>
@@ -4008,7 +3963,7 @@
         <v>16800000</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:9">
       <c r="A172" s="1" t="s">
         <v>4</v>
       </c>
@@ -4027,9 +3982,9 @@
       <c r="F172" s="9">
         <v>16800000</v>
       </c>
-      <c r="G172" s="16"/>
-    </row>
-    <row r="173" spans="1:7">
+      <c r="G172" s="15"/>
+    </row>
+    <row r="173" spans="1:9">
       <c r="A173" s="1" t="s">
         <v>4</v>
       </c>
@@ -4039,17 +3994,20 @@
       <c r="C173" s="1">
         <v>3</v>
       </c>
-      <c r="D173" s="16">
+      <c r="D173" s="12">
         <v>13400000</v>
       </c>
-      <c r="E173" s="16">
+      <c r="E173" s="12">
         <v>7000000</v>
       </c>
-      <c r="F173" s="16">
+      <c r="F173" s="12">
         <v>18000000</v>
       </c>
-    </row>
-    <row r="174" spans="1:7">
+      <c r="G173" s="15"/>
+      <c r="H173" s="15"/>
+      <c r="I173" s="15"/>
+    </row>
+    <row r="174" spans="1:9">
       <c r="A174" s="1" t="s">
         <v>5</v>
       </c>
@@ -4069,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:9">
       <c r="A175" s="1" t="s">
         <v>5</v>
       </c>
@@ -4089,7 +4047,7 @@
         <v>10700000</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:9">
       <c r="A176" s="1" t="s">
         <v>5</v>
       </c>
@@ -4879,12 +4837,16 @@
       <c r="C215" s="1">
         <v>2</v>
       </c>
-      <c r="D215" s="9"/>
-      <c r="E215" s="9"/>
-      <c r="F215" s="9"/>
-      <c r="G215" t="s">
-        <v>24</v>
-      </c>
+      <c r="D215" s="9">
+        <v>18200000</v>
+      </c>
+      <c r="E215" s="9">
+        <v>10200000</v>
+      </c>
+      <c r="F215" s="9">
+        <v>20000000</v>
+      </c>
+      <c r="G215" s="16"/>
     </row>
     <row r="216" spans="1:7">
       <c r="A216" s="1" t="s">
@@ -4896,12 +4858,16 @@
       <c r="C216" s="1">
         <v>3</v>
       </c>
-      <c r="D216" s="9"/>
-      <c r="E216" s="9"/>
-      <c r="F216" s="9"/>
-      <c r="G216" s="15" t="s">
-        <v>35</v>
-      </c>
+      <c r="D216" s="9">
+        <v>18700000</v>
+      </c>
+      <c r="E216" s="9">
+        <v>11100000</v>
+      </c>
+      <c r="F216" s="9">
+        <v>20800000</v>
+      </c>
+      <c r="G216" s="15"/>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="1" t="s">
@@ -5733,12 +5699,16 @@
       <c r="C258" s="1">
         <v>2</v>
       </c>
-      <c r="D258" s="9"/>
-      <c r="E258" s="9"/>
-      <c r="F258" s="9"/>
-      <c r="G258" t="s">
-        <v>25</v>
-      </c>
+      <c r="D258" s="9">
+        <v>26100000</v>
+      </c>
+      <c r="E258" s="9">
+        <v>16000000</v>
+      </c>
+      <c r="F258" s="9">
+        <v>32100000</v>
+      </c>
+      <c r="G258" s="16"/>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="1" t="s">
@@ -5750,12 +5720,16 @@
       <c r="C259" s="1">
         <v>3</v>
       </c>
-      <c r="D259" s="9"/>
-      <c r="E259" s="9"/>
-      <c r="F259" s="9"/>
-      <c r="G259" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="D259" s="9">
+        <v>26900000</v>
+      </c>
+      <c r="E259" s="9">
+        <v>18400000</v>
+      </c>
+      <c r="F259" s="9">
+        <v>32000000</v>
+      </c>
+      <c r="G259" s="15"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="1" t="s">
@@ -6587,12 +6561,16 @@
       <c r="C301" s="1">
         <v>2</v>
       </c>
-      <c r="D301" s="9"/>
-      <c r="E301" s="9"/>
-      <c r="F301" s="9"/>
-      <c r="G301" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="D301" s="9">
+        <v>45400000</v>
+      </c>
+      <c r="E301" s="9">
+        <v>25000000</v>
+      </c>
+      <c r="F301" s="9">
+        <v>60000000</v>
+      </c>
+      <c r="G301" s="15"/>
     </row>
     <row r="302" spans="1:7">
       <c r="A302" s="1" t="s">
@@ -6604,12 +6582,16 @@
       <c r="C302" s="1">
         <v>3</v>
       </c>
-      <c r="D302" s="9"/>
-      <c r="E302" s="9"/>
-      <c r="F302" s="9"/>
-      <c r="G302" s="15" t="s">
-        <v>37</v>
-      </c>
+      <c r="D302" s="9">
+        <v>46900000</v>
+      </c>
+      <c r="E302" s="9">
+        <v>30000000</v>
+      </c>
+      <c r="F302" s="9">
+        <v>60000000</v>
+      </c>
+      <c r="G302" s="15"/>
     </row>
     <row r="303" spans="1:7">
       <c r="A303" s="1" t="s">
@@ -7441,12 +7423,16 @@
       <c r="C344" s="1">
         <v>2</v>
       </c>
-      <c r="D344" s="9"/>
-      <c r="E344" s="9"/>
-      <c r="F344" s="9"/>
-      <c r="G344" t="s">
-        <v>27</v>
-      </c>
+      <c r="D344" s="9">
+        <v>36900000</v>
+      </c>
+      <c r="E344" s="9">
+        <v>22400000</v>
+      </c>
+      <c r="F344" s="9">
+        <v>48000000</v>
+      </c>
+      <c r="G344" s="16"/>
     </row>
     <row r="345" spans="1:7">
       <c r="A345" s="1" t="s">
@@ -7458,12 +7444,16 @@
       <c r="C345" s="1">
         <v>3</v>
       </c>
-      <c r="D345" s="9"/>
-      <c r="E345" s="9"/>
-      <c r="F345" s="9"/>
-      <c r="G345" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="D345" s="9">
+        <v>36200000</v>
+      </c>
+      <c r="E345" s="9">
+        <v>23000000</v>
+      </c>
+      <c r="F345" s="9">
+        <v>48000000</v>
+      </c>
+      <c r="G345" s="15"/>
     </row>
     <row r="346" spans="1:7">
       <c r="A346" s="1" t="s">
@@ -8315,12 +8305,16 @@
       <c r="C388" s="1">
         <v>3</v>
       </c>
-      <c r="D388" s="9"/>
-      <c r="E388" s="9"/>
-      <c r="F388" s="9"/>
-      <c r="G388" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="D388" s="9">
+        <v>28500000</v>
+      </c>
+      <c r="E388" s="9">
+        <v>15000000</v>
+      </c>
+      <c r="F388" s="9">
+        <v>35000000</v>
+      </c>
+      <c r="G388" s="15"/>
     </row>
     <row r="389" spans="1:7">
       <c r="A389" s="1" t="s">
@@ -8882,7 +8876,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="417" spans="1:7">
+    <row r="417" spans="1:9">
       <c r="A417" s="1" t="s">
         <v>10</v>
       </c>
@@ -8902,7 +8896,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="418" spans="1:7">
+    <row r="418" spans="1:9">
       <c r="A418" s="1" t="s">
         <v>10</v>
       </c>
@@ -8922,7 +8916,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="419" spans="1:7">
+    <row r="419" spans="1:9">
       <c r="A419" s="1" t="s">
         <v>10</v>
       </c>
@@ -8942,7 +8936,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="420" spans="1:7">
+    <row r="420" spans="1:9">
       <c r="A420" s="1" t="s">
         <v>10</v>
       </c>
@@ -8962,7 +8956,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="421" spans="1:7">
+    <row r="421" spans="1:9">
       <c r="A421" s="1" t="s">
         <v>10</v>
       </c>
@@ -8982,7 +8976,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="422" spans="1:7">
+    <row r="422" spans="1:9">
       <c r="A422" s="1" t="s">
         <v>10</v>
       </c>
@@ -9002,7 +8996,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:9">
       <c r="A423" s="1" t="s">
         <v>10</v>
       </c>
@@ -9022,7 +9016,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="424" spans="1:7">
+    <row r="424" spans="1:9">
       <c r="A424" s="1" t="s">
         <v>10</v>
       </c>
@@ -9042,7 +9036,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="425" spans="1:7">
+    <row r="425" spans="1:9">
       <c r="A425" s="1" t="s">
         <v>10</v>
       </c>
@@ -9062,7 +9056,7 @@
         <v>144000000</v>
       </c>
     </row>
-    <row r="426" spans="1:7">
+    <row r="426" spans="1:9">
       <c r="A426" s="1" t="s">
         <v>10</v>
       </c>
@@ -9082,7 +9076,7 @@
         <v>144000000</v>
       </c>
     </row>
-    <row r="427" spans="1:7">
+    <row r="427" spans="1:9">
       <c r="A427" s="1" t="s">
         <v>10</v>
       </c>
@@ -9102,7 +9096,7 @@
         <v>144000000</v>
       </c>
     </row>
-    <row r="428" spans="1:7">
+    <row r="428" spans="1:9">
       <c r="A428" s="1" t="s">
         <v>10</v>
       </c>
@@ -9122,7 +9116,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:9">
       <c r="A429" s="1" t="s">
         <v>10</v>
       </c>
@@ -9142,7 +9136,7 @@
         <v>137100000</v>
       </c>
     </row>
-    <row r="430" spans="1:7">
+    <row r="430" spans="1:9">
       <c r="A430" s="1" t="s">
         <v>10</v>
       </c>
@@ -9152,18 +9146,20 @@
       <c r="C430" s="1">
         <v>2</v>
       </c>
-      <c r="D430" s="9">
+      <c r="D430" s="12">
         <v>111200000</v>
       </c>
-      <c r="E430" s="16">
+      <c r="E430" s="12">
         <v>80000000</v>
       </c>
-      <c r="F430" s="9">
+      <c r="F430" s="12">
         <v>137100000</v>
       </c>
-      <c r="G430" s="17"/>
-    </row>
-    <row r="431" spans="1:7">
+      <c r="G430" s="9"/>
+      <c r="H430" s="15"/>
+      <c r="I430" s="9"/>
+    </row>
+    <row r="431" spans="1:9">
       <c r="A431" s="1" t="s">
         <v>10</v>
       </c>
@@ -9173,17 +9169,20 @@
       <c r="C431" s="1">
         <v>3</v>
       </c>
-      <c r="D431" s="16">
+      <c r="D431" s="12">
         <v>111100000</v>
       </c>
-      <c r="E431" s="16">
+      <c r="E431" s="12">
         <v>88000000</v>
       </c>
-      <c r="F431" s="16">
+      <c r="F431" s="12">
         <v>132000000</v>
       </c>
-    </row>
-    <row r="432" spans="1:7">
+      <c r="G431" s="15"/>
+      <c r="H431" s="15"/>
+      <c r="I431" s="15"/>
+    </row>
+    <row r="432" spans="1:9">
       <c r="A432" s="1" t="s">
         <v>11</v>
       </c>
@@ -10013,12 +10012,16 @@
       <c r="C473" s="1">
         <v>2</v>
       </c>
-      <c r="D473" s="9"/>
-      <c r="E473" s="9"/>
-      <c r="F473" s="9"/>
-      <c r="G473" t="s">
-        <v>28</v>
-      </c>
+      <c r="D473" s="9">
+        <v>37200000</v>
+      </c>
+      <c r="E473" s="9">
+        <v>22000000</v>
+      </c>
+      <c r="F473" s="9">
+        <v>45400000</v>
+      </c>
+      <c r="G473" s="16"/>
     </row>
     <row r="474" spans="1:7">
       <c r="A474" s="1" t="s">
@@ -10030,12 +10033,16 @@
       <c r="C474" s="1">
         <v>3</v>
       </c>
-      <c r="D474" s="9"/>
-      <c r="E474" s="9"/>
-      <c r="F474" s="9"/>
-      <c r="G474" s="15" t="s">
-        <v>40</v>
-      </c>
+      <c r="D474" s="9">
+        <v>38100000</v>
+      </c>
+      <c r="E474" s="9">
+        <v>22600000</v>
+      </c>
+      <c r="F474" s="9">
+        <v>45000000</v>
+      </c>
+      <c r="G474" s="15"/>
     </row>
     <row r="475" spans="1:7">
       <c r="A475" s="1" t="s">
@@ -10797,7 +10804,7 @@
         <v>38000000</v>
       </c>
     </row>
-    <row r="513" spans="1:7">
+    <row r="513" spans="1:8">
       <c r="A513" s="1" t="s">
         <v>12</v>
       </c>
@@ -10817,7 +10824,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="514" spans="1:7">
+    <row r="514" spans="1:8">
       <c r="A514" s="1" t="s">
         <v>12</v>
       </c>
@@ -10837,7 +10844,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="515" spans="1:7">
+    <row r="515" spans="1:8">
       <c r="A515" s="1" t="s">
         <v>12</v>
       </c>
@@ -10857,7 +10864,7 @@
         <v>42000000</v>
       </c>
     </row>
-    <row r="516" spans="1:7">
+    <row r="516" spans="1:8">
       <c r="A516" s="1" t="s">
         <v>12</v>
       </c>
@@ -10867,16 +10874,19 @@
       <c r="C516" s="1">
         <v>2</v>
       </c>
-      <c r="D516" s="16">
+      <c r="D516" s="12">
         <v>40000000</v>
       </c>
-      <c r="E516" s="9"/>
-      <c r="F516" s="9"/>
-      <c r="G516" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="517" spans="1:7">
+      <c r="E516" s="9">
+        <v>30000000</v>
+      </c>
+      <c r="F516" s="12">
+        <v>42000000</v>
+      </c>
+      <c r="G516" s="15"/>
+      <c r="H516" s="15"/>
+    </row>
+    <row r="517" spans="1:8">
       <c r="A517" s="1" t="s">
         <v>12</v>
       </c>
@@ -10886,16 +10896,19 @@
       <c r="C517" s="1">
         <v>3</v>
       </c>
-      <c r="D517" s="16">
+      <c r="D517" s="12">
         <v>39900000</v>
       </c>
-      <c r="E517" s="9"/>
-      <c r="F517" s="9"/>
-      <c r="G517" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="518" spans="1:7">
+      <c r="E517" s="9">
+        <v>32000000</v>
+      </c>
+      <c r="F517" s="12">
+        <v>42000000</v>
+      </c>
+      <c r="G517" s="15"/>
+      <c r="H517" s="15"/>
+    </row>
+    <row r="518" spans="1:8">
       <c r="A518" s="1" t="s">
         <v>13</v>
       </c>
@@ -10915,7 +10928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="519" spans="1:7">
+    <row r="519" spans="1:8">
       <c r="A519" s="1" t="s">
         <v>13</v>
       </c>
@@ -10935,7 +10948,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="520" spans="1:7">
+    <row r="520" spans="1:8">
       <c r="A520" s="1" t="s">
         <v>13</v>
       </c>
@@ -10955,7 +10968,7 @@
         <v>19500000</v>
       </c>
     </row>
-    <row r="521" spans="1:7">
+    <row r="521" spans="1:8">
       <c r="A521" s="1" t="s">
         <v>13</v>
       </c>
@@ -10975,7 +10988,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="522" spans="1:7">
+    <row r="522" spans="1:8">
       <c r="A522" s="1" t="s">
         <v>13</v>
       </c>
@@ -10995,7 +11008,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="523" spans="1:7">
+    <row r="523" spans="1:8">
       <c r="A523" s="1" t="s">
         <v>13</v>
       </c>
@@ -11015,7 +11028,7 @@
         <v>24000000</v>
       </c>
     </row>
-    <row r="524" spans="1:7">
+    <row r="524" spans="1:8">
       <c r="A524" s="1" t="s">
         <v>13</v>
       </c>
@@ -11035,7 +11048,7 @@
         <v>26000000</v>
       </c>
     </row>
-    <row r="525" spans="1:7">
+    <row r="525" spans="1:8">
       <c r="A525" s="1" t="s">
         <v>13</v>
       </c>
@@ -11055,7 +11068,7 @@
         <v>26000000</v>
       </c>
     </row>
-    <row r="526" spans="1:7">
+    <row r="526" spans="1:8">
       <c r="A526" s="1" t="s">
         <v>13</v>
       </c>
@@ -11075,7 +11088,7 @@
         <v>27500000</v>
       </c>
     </row>
-    <row r="527" spans="1:7">
+    <row r="527" spans="1:8">
       <c r="A527" s="1" t="s">
         <v>13</v>
       </c>
@@ -11095,7 +11108,7 @@
         <v>27000000</v>
       </c>
     </row>
-    <row r="528" spans="1:7">
+    <row r="528" spans="1:8">
       <c r="A528" s="1" t="s">
         <v>13</v>
       </c>
@@ -11435,7 +11448,7 @@
         <v>26800000</v>
       </c>
     </row>
-    <row r="545" spans="1:7">
+    <row r="545" spans="1:8">
       <c r="A545" s="1" t="s">
         <v>13</v>
       </c>
@@ -11455,7 +11468,7 @@
         <v>26800000</v>
       </c>
     </row>
-    <row r="546" spans="1:7">
+    <row r="546" spans="1:8">
       <c r="A546" s="1" t="s">
         <v>13</v>
       </c>
@@ -11475,7 +11488,7 @@
         <v>28600000</v>
       </c>
     </row>
-    <row r="547" spans="1:7">
+    <row r="547" spans="1:8">
       <c r="A547" s="1" t="s">
         <v>13</v>
       </c>
@@ -11495,7 +11508,7 @@
         <v>27800000</v>
       </c>
     </row>
-    <row r="548" spans="1:7">
+    <row r="548" spans="1:8">
       <c r="A548" s="1" t="s">
         <v>13</v>
       </c>
@@ -11515,7 +11528,7 @@
         <v>29800000</v>
       </c>
     </row>
-    <row r="549" spans="1:7">
+    <row r="549" spans="1:8">
       <c r="A549" s="1" t="s">
         <v>13</v>
       </c>
@@ -11535,7 +11548,7 @@
         <v>29700000</v>
       </c>
     </row>
-    <row r="550" spans="1:7">
+    <row r="550" spans="1:8">
       <c r="A550" s="1" t="s">
         <v>13</v>
       </c>
@@ -11555,7 +11568,7 @@
         <v>29700000</v>
       </c>
     </row>
-    <row r="551" spans="1:7">
+    <row r="551" spans="1:8">
       <c r="A551" s="1" t="s">
         <v>13</v>
       </c>
@@ -11575,7 +11588,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="552" spans="1:7">
+    <row r="552" spans="1:8">
       <c r="A552" s="1" t="s">
         <v>13</v>
       </c>
@@ -11595,7 +11608,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="553" spans="1:7">
+    <row r="553" spans="1:8">
       <c r="A553" s="1" t="s">
         <v>13</v>
       </c>
@@ -11615,7 +11628,7 @@
         <v>32000000</v>
       </c>
     </row>
-    <row r="554" spans="1:7">
+    <row r="554" spans="1:8">
       <c r="A554" s="1" t="s">
         <v>13</v>
       </c>
@@ -11635,7 +11648,7 @@
         <v>31700000</v>
       </c>
     </row>
-    <row r="555" spans="1:7">
+    <row r="555" spans="1:8">
       <c r="A555" s="1" t="s">
         <v>13</v>
       </c>
@@ -11655,7 +11668,7 @@
         <v>31400000</v>
       </c>
     </row>
-    <row r="556" spans="1:7">
+    <row r="556" spans="1:8">
       <c r="A556" s="1" t="s">
         <v>13</v>
       </c>
@@ -11675,7 +11688,7 @@
         <v>32000000</v>
       </c>
     </row>
-    <row r="557" spans="1:7">
+    <row r="557" spans="1:8">
       <c r="A557" s="1" t="s">
         <v>13</v>
       </c>
@@ -11695,7 +11708,7 @@
         <v>32000000</v>
       </c>
     </row>
-    <row r="558" spans="1:7">
+    <row r="558" spans="1:8">
       <c r="A558" s="1" t="s">
         <v>13</v>
       </c>
@@ -11715,7 +11728,7 @@
         <v>34000000</v>
       </c>
     </row>
-    <row r="559" spans="1:7">
+    <row r="559" spans="1:8">
       <c r="A559" s="1" t="s">
         <v>13</v>
       </c>
@@ -11725,16 +11738,19 @@
       <c r="C559" s="1">
         <v>2</v>
       </c>
-      <c r="D559" s="16">
+      <c r="D559" s="12">
         <v>30100000</v>
       </c>
-      <c r="E559" s="9"/>
-      <c r="F559" s="9"/>
-      <c r="G559" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="560" spans="1:7">
+      <c r="E559" s="9">
+        <v>19800000</v>
+      </c>
+      <c r="F559" s="12">
+        <v>34000000</v>
+      </c>
+      <c r="G559" s="15"/>
+      <c r="H559" s="15"/>
+    </row>
+    <row r="560" spans="1:8">
       <c r="A560" s="1" t="s">
         <v>13</v>
       </c>
@@ -11744,14 +11760,17 @@
       <c r="C560" s="1">
         <v>3</v>
       </c>
-      <c r="D560" s="16">
+      <c r="D560" s="12">
         <v>30200000</v>
       </c>
-      <c r="E560" s="9"/>
-      <c r="F560" s="9"/>
-      <c r="G560" s="15" t="s">
-        <v>42</v>
-      </c>
+      <c r="E560" s="9">
+        <v>19800000</v>
+      </c>
+      <c r="F560" s="12">
+        <v>33000000</v>
+      </c>
+      <c r="G560" s="15"/>
+      <c r="H560" s="15"/>
     </row>
     <row r="561" spans="1:6">
       <c r="A561" s="1" t="s">
@@ -12393,7 +12412,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="593" spans="1:7">
+    <row r="593" spans="1:9">
       <c r="A593" s="1" t="s">
         <v>14</v>
       </c>
@@ -12413,7 +12432,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="594" spans="1:7">
+    <row r="594" spans="1:9">
       <c r="A594" s="1" t="s">
         <v>14</v>
       </c>
@@ -12433,7 +12452,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="595" spans="1:7">
+    <row r="595" spans="1:9">
       <c r="A595" s="1" t="s">
         <v>14</v>
       </c>
@@ -12453,7 +12472,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="596" spans="1:7">
+    <row r="596" spans="1:9">
       <c r="A596" s="1" t="s">
         <v>14</v>
       </c>
@@ -12473,7 +12492,7 @@
         <v>36800000</v>
       </c>
     </row>
-    <row r="597" spans="1:7">
+    <row r="597" spans="1:9">
       <c r="A597" s="1" t="s">
         <v>14</v>
       </c>
@@ -12493,7 +12512,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="598" spans="1:7">
+    <row r="598" spans="1:9">
       <c r="A598" s="1" t="s">
         <v>14</v>
       </c>
@@ -12513,7 +12532,7 @@
         <v>37000000</v>
       </c>
     </row>
-    <row r="599" spans="1:7">
+    <row r="599" spans="1:9">
       <c r="A599" s="1" t="s">
         <v>14</v>
       </c>
@@ -12533,7 +12552,7 @@
         <v>38000000</v>
       </c>
     </row>
-    <row r="600" spans="1:7">
+    <row r="600" spans="1:9">
       <c r="A600" s="1" t="s">
         <v>14</v>
       </c>
@@ -12553,7 +12572,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="601" spans="1:7">
+    <row r="601" spans="1:9">
       <c r="A601" s="1" t="s">
         <v>14</v>
       </c>
@@ -12563,17 +12582,20 @@
       <c r="C601" s="1">
         <v>1</v>
       </c>
-      <c r="D601" s="14">
+      <c r="D601" s="12">
         <v>34500000</v>
       </c>
-      <c r="E601" s="14">
+      <c r="E601" s="12">
         <v>25000000</v>
       </c>
-      <c r="F601" s="14">
+      <c r="F601" s="12">
         <v>37900000</v>
       </c>
-    </row>
-    <row r="602" spans="1:7">
+      <c r="G601" s="14"/>
+      <c r="H601" s="14"/>
+      <c r="I601" s="14"/>
+    </row>
+    <row r="602" spans="1:9">
       <c r="A602" s="1" t="s">
         <v>14</v>
       </c>
@@ -12583,16 +12605,19 @@
       <c r="C602" s="1">
         <v>2</v>
       </c>
-      <c r="D602" s="16">
+      <c r="D602" s="12">
         <v>34900000</v>
       </c>
-      <c r="E602" s="1"/>
-      <c r="F602" s="1"/>
-      <c r="G602" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="603" spans="1:7">
+      <c r="E602" s="12">
+        <v>25000000</v>
+      </c>
+      <c r="F602" s="12">
+        <v>37900000</v>
+      </c>
+      <c r="G602" s="15"/>
+      <c r="H602" s="15"/>
+    </row>
+    <row r="603" spans="1:9">
       <c r="A603" s="1" t="s">
         <v>14</v>
       </c>
@@ -12602,16 +12627,19 @@
       <c r="C603" s="1">
         <v>3</v>
       </c>
-      <c r="D603" s="16">
+      <c r="D603" s="12">
         <v>34800000</v>
       </c>
-      <c r="E603" s="1"/>
-      <c r="F603" s="1"/>
-      <c r="G603" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="604" spans="1:7">
+      <c r="E603" s="12">
+        <v>27000000</v>
+      </c>
+      <c r="F603" s="12">
+        <v>40000000</v>
+      </c>
+      <c r="G603" s="15"/>
+      <c r="H603" s="15"/>
+    </row>
+    <row r="604" spans="1:9">
       <c r="A604" s="1"/>
       <c r="B604" s="1"/>
       <c r="C604" s="1"/>
@@ -12619,7 +12647,7 @@
       <c r="E604" s="1"/>
       <c r="F604" s="1"/>
     </row>
-    <row r="605" spans="1:7">
+    <row r="605" spans="1:9">
       <c r="A605" s="1"/>
       <c r="B605" s="1"/>
       <c r="C605" s="1"/>
@@ -12627,7 +12655,7 @@
       <c r="E605" s="1"/>
       <c r="F605" s="1"/>
     </row>
-    <row r="606" spans="1:7">
+    <row r="606" spans="1:9">
       <c r="A606" s="1"/>
       <c r="B606" s="1"/>
       <c r="C606" s="1"/>
@@ -12635,7 +12663,7 @@
       <c r="E606" s="1"/>
       <c r="F606" s="1"/>
     </row>
-    <row r="607" spans="1:7">
+    <row r="607" spans="1:9">
       <c r="A607" s="1"/>
       <c r="B607" s="1"/>
       <c r="C607" s="1"/>

</xml_diff>